<commit_message>
doc: add GR08_ALU_DEEP test
</commit_message>
<xml_diff>
--- a/TFT_Coordination.xlsx
+++ b/TFT_Coordination.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>G04</t>
   </si>
@@ -80,7 +80,10 @@
     <t>FORWARDING_STALL_JUMPS()</t>
   </si>
   <si>
-    <t>Covered</t>
+    <t>TESTED</t>
+  </si>
+  <si>
+    <t>SIMULATED. NOT TESTED</t>
   </si>
 </sst>
 </file>
@@ -124,7 +127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -136,6 +139,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -418,8 +424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F5:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F3" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="G3" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,7 +436,7 @@
     <col min="9" max="9" width="20.5703125" customWidth="1"/>
     <col min="10" max="10" width="32.7109375" customWidth="1"/>
     <col min="11" max="11" width="16.28515625" customWidth="1"/>
-    <col min="12" max="12" width="18" customWidth="1"/>
+    <col min="12" max="12" width="23.140625" customWidth="1"/>
     <col min="13" max="13" width="21.28515625" customWidth="1"/>
     <col min="14" max="14" width="15.28515625" customWidth="1"/>
     <col min="15" max="15" width="14.7109375" customWidth="1"/>
@@ -485,6 +491,9 @@
       <c r="K7" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="L7" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="8" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F8" s="1" t="s">
@@ -505,11 +514,15 @@
       <c r="F11" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="L11" s="4"/>
     </row>
     <row r="12" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F12" s="1" t="s">
         <v>6</v>
       </c>
+    </row>
+    <row r="13" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="L13" s="4"/>
     </row>
     <row r="14" spans="6:17" x14ac:dyDescent="0.25">
       <c r="J14" s="4"/>

</xml_diff>

<commit_message>
Update Excel File for G04
</commit_message>
<xml_diff>
--- a/TFT_Coordination.xlsx
+++ b/TFT_Coordination.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lorenzo\Documents\Universit\magistrale\Testing and fault tolerance\GitContest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Iman\Dropbox (Personal)\Master_CE_Polito\Term 3\Testing and fault tolerance (8)\Laboratory\Contest\Project\Testing-Contest\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6005BD-6122-4259-AFAB-E3EB8BFC331C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>G04</t>
   </si>
@@ -81,12 +82,15 @@
   </si>
   <si>
     <t>TESTED</t>
+  </si>
+  <si>
+    <t>all done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -145,7 +149,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -422,30 +426,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="F5:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G3" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="28.42578125" customWidth="1"/>
-    <col min="7" max="7" width="30.85546875" customWidth="1"/>
-    <col min="8" max="8" width="25.28515625" customWidth="1"/>
-    <col min="9" max="9" width="20.5703125" customWidth="1"/>
-    <col min="10" max="10" width="32.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" customWidth="1"/>
-    <col min="12" max="12" width="23.140625" customWidth="1"/>
-    <col min="13" max="13" width="21.28515625" customWidth="1"/>
-    <col min="14" max="14" width="15.28515625" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" customWidth="1"/>
-    <col min="16" max="16" width="20.5703125" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="28.44140625" customWidth="1"/>
+    <col min="7" max="7" width="30.88671875" customWidth="1"/>
+    <col min="8" max="8" width="25.33203125" customWidth="1"/>
+    <col min="9" max="9" width="20.5546875" customWidth="1"/>
+    <col min="10" max="10" width="32.6640625" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" customWidth="1"/>
+    <col min="12" max="12" width="23.109375" customWidth="1"/>
+    <col min="13" max="13" width="21.33203125" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" customWidth="1"/>
+    <col min="15" max="15" width="14.6640625" customWidth="1"/>
+    <col min="16" max="16" width="20.5546875" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="6:17" x14ac:dyDescent="0.3">
       <c r="G5" s="2" t="s">
         <v>17</v>
       </c>
@@ -480,12 +484,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="6:17" x14ac:dyDescent="0.3">
       <c r="F6" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="6:17" x14ac:dyDescent="0.3">
       <c r="F7" s="1" t="s">
         <v>1</v>
       </c>
@@ -499,36 +506,36 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="6:17" x14ac:dyDescent="0.3">
       <c r="F8" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="6:17" x14ac:dyDescent="0.3">
       <c r="F9" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="6:17" x14ac:dyDescent="0.3">
       <c r="F10" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="6:17" x14ac:dyDescent="0.3">
       <c r="F11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="L11" s="6"/>
     </row>
-    <row r="12" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="6:17" x14ac:dyDescent="0.3">
       <c r="F12" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="6:17" x14ac:dyDescent="0.3">
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="6:17" x14ac:dyDescent="0.3">
       <c r="J14" s="4"/>
     </row>
   </sheetData>

</xml_diff>